<commit_message>
end of lab 2 commits - aircraft NPX
</commit_message>
<xml_diff>
--- a/data/Preprocessed Data/Intermediates/CSV [DEC2HEX]/scratch.xlsx
+++ b/data/Preprocessed Data/Intermediates/CSV [DEC2HEX]/scratch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosmo\Documents\TCD\Processing\High5ive\data\Preprocessed Data\Intermediates\CSV [DEC2HEX]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24825CAA-26AA-4CA3-AE00-205599568481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4612DAE9-82D4-4215-81B4-49BC6D35BDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,14 +348,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="S2:AJ2"/>
+  <dimension ref="S1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="19:36" x14ac:dyDescent="0.25">
+      <c r="S1">
+        <f>ROUND(CONVERT(R1,"mi","km"),0)</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="19:36" x14ac:dyDescent="0.25">
       <c r="S2" t="str">
         <f>DEC2HEX(A2,2)</f>

</xml_diff>